<commit_message>
pb data fix, optim pso+asd
</commit_message>
<xml_diff>
--- a/carbomica_framework.xlsx
+++ b/carbomica_framework.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="108">
   <si>
     <t>Name</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>Targetable</t>
+  </si>
+  <si>
+    <t>Unnamed: 12</t>
+  </si>
+  <si>
+    <t>Unnamed: 13</t>
   </si>
   <si>
     <t>co2e_emissions</t>
@@ -876,13 +882,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -920,32 +926,38 @@
         <v>23</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I3" t="s">
         <v>28</v>
@@ -954,12 +966,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -971,35 +983,35 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="K4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I5" t="s">
         <v>28</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I6" t="s">
         <v>28</v>
@@ -1008,12 +1020,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1025,35 +1037,35 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="K7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I8" t="s">
         <v>28</v>
       </c>
-      <c r="M8" t="s">
+      <c r="O8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I9" t="s">
         <v>28</v>
@@ -1062,12 +1074,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1079,35 +1091,35 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="K10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H11" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I11" t="s">
         <v>28</v>
       </c>
-      <c r="M11" t="s">
+      <c r="O11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I12" t="s">
         <v>28</v>
@@ -1116,12 +1128,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1133,35 +1145,35 @@
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="K13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H14" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I14" t="s">
         <v>28</v>
       </c>
-      <c r="M14" t="s">
+      <c r="O14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I15" t="s">
         <v>28</v>
@@ -1170,12 +1182,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1187,35 +1199,35 @@
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="K16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H17" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I17" t="s">
         <v>28</v>
       </c>
-      <c r="M17" t="s">
+      <c r="O17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I18" t="s">
         <v>28</v>
@@ -1224,12 +1236,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1241,35 +1253,35 @@
         <v>1</v>
       </c>
       <c r="I19" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="K19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H20" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I20" t="s">
         <v>28</v>
       </c>
-      <c r="M20" t="s">
+      <c r="O20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I21" t="s">
         <v>28</v>
@@ -1278,12 +1290,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1295,35 +1307,35 @@
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="K22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H23" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I23" t="s">
         <v>28</v>
       </c>
-      <c r="M23" t="s">
+      <c r="O23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I24" t="s">
         <v>28</v>
@@ -1332,12 +1344,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1349,26 +1361,26 @@
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="K25" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:15">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H26" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="I26" t="s">
         <v>28</v>
       </c>
-      <c r="M26" t="s">
+      <c r="O26" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1393,10 +1405,10 @@
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>32</v>
@@ -1435,10 +1447,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1462,16 +1474,16 @@
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>